<commit_message>
Check for end-of-file rather than detecting 99 at the end of the file. Print out test vector file name.
</commit_message>
<xml_diff>
--- a/Date_calculator_console_app/date_test_data_04_w_notes.xlsx
+++ b/Date_calculator_console_app/date_test_data_04_w_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\git_repositories\Date_calculator_console_app\Date_calculator_console_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B007B3-8EA6-4935-9656-D53EA492F4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EABD52-46F8-40A2-84E9-D2686D8748CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37470" yWindow="1920" windowWidth="18615" windowHeight="13515" xr2:uid="{227263D0-AED4-45ED-8ED9-036391BA46B7}"/>
+    <workbookView xWindow="37110" yWindow="1020" windowWidth="18615" windowHeight="13515" xr2:uid="{227263D0-AED4-45ED-8ED9-036391BA46B7}"/>
   </bookViews>
   <sheets>
     <sheet name="date_test_data_01" sheetId="1" r:id="rId1"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DABDEE-2000-4FEC-878E-9C98AAD9B175}">
   <dimension ref="A1:M276"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>